<commit_message>
Added Flexjson. Removed some libs from Excel result.
It seems that Boon doesnt have extendable parser.
And Alibaba doesn't seem to have extensions at all.
Flexjson fails on UUID ;(
Jil fails on non-trivial stuff ;(

TODO: rerun bench
</commit_message>
<xml_diff>
--- a/GatherResults/template.xlsx
+++ b/GatherResults/template.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="66">
   <si>
     <t>Serialization</t>
   </si>
@@ -55,12 +55,6 @@
     <t>Service Stack</t>
   </si>
   <si>
-    <t>Boon</t>
-  </si>
-  <si>
-    <t>Alibaba</t>
-  </si>
-  <si>
     <t>Instance + serialization + deserialization:</t>
   </si>
   <si>
@@ -103,12 +97,6 @@
     <t>[[instance.DslJava.Duration]]</t>
   </si>
   <si>
-    <t>[[instance.Boon.Duration]]</t>
-  </si>
-  <si>
-    <t>[[instance.Alibaba.Duration]]</t>
-  </si>
-  <si>
     <t>[[instance.Gson.Duration]]</t>
   </si>
   <si>
@@ -130,12 +118,6 @@
     <t>[[both.DslJava.Duration]]</t>
   </si>
   <si>
-    <t>[[both.Boon.Duration]]</t>
-  </si>
-  <si>
-    <t>[[both.Alibaba.Duration]]</t>
-  </si>
-  <si>
     <t>[[both.Gson.Duration]]</t>
   </si>
   <si>
@@ -172,12 +154,6 @@
     <t>[[serialization.DslJava.Duration]]</t>
   </si>
   <si>
-    <t>[[serialization.Boon.Duration]]</t>
-  </si>
-  <si>
-    <t>[[serialization.Alibaba.Duration]]</t>
-  </si>
-  <si>
     <t>[[serialization.Gson.Duration]]</t>
   </si>
   <si>
@@ -187,12 +163,6 @@
     <t>[[serialization.DslJava.Size]]</t>
   </si>
   <si>
-    <t>Boon (size)</t>
-  </si>
-  <si>
-    <t>[[serialization.Boon.Size]]</t>
-  </si>
-  <si>
     <t>[[serialization.NetJSON.Size]]</t>
   </si>
   <si>
@@ -205,18 +175,12 @@
     <t>[[serialization.Jil.Duration]]</t>
   </si>
   <si>
-    <t>Alibaba (size)</t>
-  </si>
-  <si>
     <t>Gson (size)</t>
   </si>
   <si>
     <t>[[serialization.Gson.Size]]</t>
   </si>
   <si>
-    <t>[[serialization.Alibaba.Size]]</t>
-  </si>
-  <si>
     <t>NetJSON</t>
   </si>
   <si>
@@ -230,6 +194,24 @@
   </si>
   <si>
     <t>Jackson afterburner</t>
+  </si>
+  <si>
+    <t>Genson</t>
+  </si>
+  <si>
+    <t>Genson (size)</t>
+  </si>
+  <si>
+    <t>[[serialization.Genson.Size]]</t>
+  </si>
+  <si>
+    <t>[[serialization.Genson.Duration]]</t>
+  </si>
+  <si>
+    <t>[[instance.Genson.Duration]]</t>
+  </si>
+  <si>
+    <t>[[both.Genson.Duration]]</t>
   </si>
 </sst>
 </file>
@@ -287,13 +269,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
-    <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.0"/>
-    </dxf>
+  <dxfs count="18">
     <dxf>
       <numFmt numFmtId="164" formatCode="#,##0.0"/>
     </dxf>
@@ -416,9 +392,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$C$37:$L$37</c:f>
+              <c:f>Sheet1!$C$37:$K$37</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>Newtonsoft</c:v>
                 </c:pt>
@@ -441,12 +417,9 @@
                   <c:v>DSL Platform Java</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Boon</c:v>
+                  <c:v>Genson</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Alibaba</c:v>
-                </c:pt>
-                <c:pt idx="9">
                   <c:v>Gson</c:v>
                 </c:pt>
               </c:strCache>
@@ -454,10 +427,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$39:$L$39</c:f>
+              <c:f>Sheet1!$C$39:$K$39</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.0</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -483,9 +456,6 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -509,9 +479,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$C$37:$L$37</c:f>
+              <c:f>Sheet1!$C$37:$K$37</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>Newtonsoft</c:v>
                 </c:pt>
@@ -534,12 +504,9 @@
                   <c:v>DSL Platform Java</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Boon</c:v>
+                  <c:v>Genson</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Alibaba</c:v>
-                </c:pt>
-                <c:pt idx="9">
                   <c:v>Gson</c:v>
                 </c:pt>
               </c:strCache>
@@ -547,10 +514,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$40:$L$40</c:f>
+              <c:f>Sheet1!$C$40:$K$40</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.0</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -576,9 +543,6 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -594,11 +558,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="62012032"/>
-        <c:axId val="62267776"/>
+        <c:axId val="114873856"/>
+        <c:axId val="114875392"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="62012032"/>
+        <c:axId val="114873856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -607,7 +571,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62267776"/>
+        <c:crossAx val="114875392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -615,7 +579,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="62267776"/>
+        <c:axId val="114875392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -646,7 +610,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62012032"/>
+        <c:crossAx val="114873856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -710,9 +674,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$C$37:$L$37</c:f>
+              <c:f>Sheet1!$C$37:$K$37</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>Newtonsoft</c:v>
                 </c:pt>
@@ -735,12 +699,9 @@
                   <c:v>DSL Platform Java</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Boon</c:v>
+                  <c:v>Genson</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Alibaba</c:v>
-                </c:pt>
-                <c:pt idx="9">
                   <c:v>Gson</c:v>
                 </c:pt>
               </c:strCache>
@@ -748,10 +709,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$42:$L$42</c:f>
+              <c:f>Sheet1!$C$42:$K$42</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -777,9 +738,6 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="#,##0.0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9" formatCode="#,##0.0">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -795,11 +753,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="42816640"/>
-        <c:axId val="42818176"/>
+        <c:axId val="114900352"/>
+        <c:axId val="114910336"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="42816640"/>
+        <c:axId val="114900352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -808,7 +766,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42818176"/>
+        <c:crossAx val="114910336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -816,7 +774,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="42818176"/>
+        <c:axId val="114910336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -847,7 +805,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42816640"/>
+        <c:crossAx val="114900352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -937,9 +895,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Serialization" displayName="Serialization" ref="B55:U56">
-  <autoFilter ref="B55:U56"/>
-  <tableColumns count="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Serialization" displayName="Serialization" ref="B55:S56">
+  <autoFilter ref="B55:S56"/>
+  <tableColumns count="18">
     <tableColumn id="2" name="Newtonsoft" totalsRowFunction="custom">
       <totalsRowFormula>AverageNumbers[](Serialization[Newtonsoft])</totalsRowFormula>
     </tableColumn>
@@ -953,8 +911,7 @@
     <tableColumn id="4" name="DSL Platform Java" totalsRowFunction="custom">
       <totalsRowFormula>AverageNumbers[](Serialization[DSL Platform Java])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="11" name="Boon"/>
-    <tableColumn id="10" name="Alibaba"/>
+    <tableColumn id="11" name="Genson"/>
     <tableColumn id="5" name="Gson" totalsRowFunction="custom">
       <totalsRowFormula>AverageNumbers[](Serialization[Gson])</totalsRowFormula>
     </tableColumn>
@@ -967,8 +924,7 @@
     <tableColumn id="12" name="NetJSON (size)"/>
     <tableColumn id="16" name="Jackson (size)"/>
     <tableColumn id="17" name="DSL Platform Java (size)"/>
-    <tableColumn id="18" name="Boon (size)"/>
-    <tableColumn id="19" name="Alibaba (size)"/>
+    <tableColumn id="18" name="Genson (size)"/>
     <tableColumn id="20" name="Gson (size)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -976,31 +932,30 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="AverageNumbers" displayName="AverageNumbers" ref="B37:L42" totalsRowShown="0">
-  <autoFilter ref="B37:L42"/>
-  <tableColumns count="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="AverageNumbers" displayName="AverageNumbers" ref="B37:K42" totalsRowShown="0">
+  <autoFilter ref="B37:K42"/>
+  <tableColumns count="10">
     <tableColumn id="1" name="Average"/>
-    <tableColumn id="2" name="Newtonsoft" dataDxfId="19">
+    <tableColumn id="2" name="Newtonsoft" dataDxfId="17">
       <calculatedColumnFormula>AverageNumbers[](Serialization[Newtonsoft])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Revenj" dataDxfId="18"/>
-    <tableColumn id="4" name="Service Stack" dataDxfId="17"/>
-    <tableColumn id="8" name="Jil" dataDxfId="16"/>
-    <tableColumn id="7" name="NetJSON" dataDxfId="15"/>
-    <tableColumn id="5" name="Jackson afterburner" dataDxfId="14"/>
-    <tableColumn id="6" name="DSL Platform Java" dataDxfId="13"/>
-    <tableColumn id="9" name="Boon" dataDxfId="12"/>
-    <tableColumn id="10" name="Alibaba" dataDxfId="11"/>
-    <tableColumn id="11" name="Gson" dataDxfId="10"/>
+    <tableColumn id="3" name="Revenj" dataDxfId="16"/>
+    <tableColumn id="4" name="Service Stack" dataDxfId="15"/>
+    <tableColumn id="8" name="Jil" dataDxfId="14"/>
+    <tableColumn id="7" name="NetJSON" dataDxfId="13"/>
+    <tableColumn id="5" name="Jackson afterburner" dataDxfId="12"/>
+    <tableColumn id="6" name="DSL Platform Java" dataDxfId="11"/>
+    <tableColumn id="9" name="Genson" dataDxfId="10"/>
+    <tableColumn id="10" name="Gson" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="DeviationNumbers" displayName="DeviationNumbers" ref="B46:L48" totalsRowShown="0">
-  <autoFilter ref="B46:L48"/>
-  <tableColumns count="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="DeviationNumbers" displayName="DeviationNumbers" ref="B46:K48" totalsRowShown="0">
+  <autoFilter ref="B46:K48"/>
+  <tableColumns count="10">
     <tableColumn id="1" name="Deviation"/>
     <tableColumn id="2" name="Newtonsoft" dataDxfId="9">
       <calculatedColumnFormula>AverageNumbers[](Serialization[Newtonsoft])</calculatedColumnFormula>
@@ -1015,18 +970,17 @@
     </tableColumn>
     <tableColumn id="7" name="Jackson afterburner" dataDxfId="4"/>
     <tableColumn id="8" name="DSL Platform Java" dataDxfId="3"/>
-    <tableColumn id="9" name="Boon" dataDxfId="2"/>
-    <tableColumn id="10" name="Alibaba" dataDxfId="1"/>
-    <tableColumn id="11" name="Gson" dataDxfId="0"/>
+    <tableColumn id="9" name="Genson" dataDxfId="2"/>
+    <tableColumn id="10" name="Gson" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Both" displayName="Both" ref="B59:K60">
-  <autoFilter ref="B59:K60"/>
-  <tableColumns count="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Both" displayName="Both" ref="B59:J60">
+  <autoFilter ref="B59:J60"/>
+  <tableColumns count="9">
     <tableColumn id="2" name="Newtonsoft" totalsRowFunction="custom">
       <totalsRowFormula>AverageNumbers[](Both[Newtonsoft])</totalsRowFormula>
     </tableColumn>
@@ -1040,8 +994,7 @@
     <tableColumn id="6" name="DSL Platform Java" totalsRowFunction="custom">
       <totalsRowFormula>AverageNumbers[](Both[DSL Platform Java])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" name="Boon"/>
-    <tableColumn id="5" name="Alibaba"/>
+    <tableColumn id="3" name="Genson"/>
     <tableColumn id="7" name="Gson"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1049,9 +1002,9 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Instance" displayName="Instance" ref="B51:K52">
-  <autoFilter ref="B51:K52"/>
-  <tableColumns count="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Instance" displayName="Instance" ref="B51:J52">
+  <autoFilter ref="B51:J52"/>
+  <tableColumns count="9">
     <tableColumn id="2" name="Newtonsoft" totalsRowFunction="custom">
       <totalsRowFormula>AverageNumbers[](Instance[Newtonsoft])</totalsRowFormula>
     </tableColumn>
@@ -1065,8 +1018,7 @@
     <tableColumn id="6" name="DSL Platform Java" totalsRowFunction="custom">
       <totalsRowFormula>AverageNumbers[](Instance[DSL Platform Java])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" name="Boon"/>
-    <tableColumn id="5" name="Alibaba"/>
+    <tableColumn id="3" name="Genson"/>
     <tableColumn id="7" name="Gson"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1360,7 +1312,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:U60"/>
+  <dimension ref="B1:S60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
@@ -1400,39 +1352,36 @@
         <v>2</v>
       </c>
       <c r="C37" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D37" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E37" t="s">
         <v>12</v>
       </c>
       <c r="F37" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="G37" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="H37" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="I37" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J37" t="s">
-        <v>13</v>
+        <v>60</v>
       </c>
       <c r="K37" t="s">
-        <v>14</v>
-      </c>
-      <c r="L37" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="C38" s="2" t="e">
         <f>AVERAGE(Instance[Newtonsoft])</f>
@@ -1463,17 +1412,14 @@
         <v>#DIV/0!</v>
       </c>
       <c r="J38" s="2" t="e">
-        <f>AVERAGE(Instance[Boon])</f>
+        <f>AVERAGE(Instance[Genson])</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K38" s="2" t="e">
-        <f>AVERAGE(Instance[Alibaba])</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L38" s="2" t="e">
         <f>AVERAGE(Instance[Gson])</f>
         <v>#DIV/0!</v>
       </c>
+      <c r="L38" s="2"/>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
     </row>
@@ -1510,17 +1456,14 @@
         <v>#DIV/0!</v>
       </c>
       <c r="J39" s="2" t="e">
-        <f>AVERAGE(Serialization[Boon]) - J38</f>
+        <f>AVERAGE(Serialization[Genson]) - J38</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K39" s="2" t="e">
-        <f>AVERAGE(Serialization[Alibaba]) - K38</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L39" s="2" t="e">
-        <f>AVERAGE(Serialization[Gson]) - L38</f>
-        <v>#DIV/0!</v>
-      </c>
+        <f>AVERAGE(Serialization[Gson]) - K38</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L39" s="2"/>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
     </row>
@@ -1549,7 +1492,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="H40" s="2" t="e">
-        <f t="shared" ref="H40:K40" si="1">H41 - H39 - H38</f>
+        <f t="shared" ref="H40" si="1">H41 - H39 - H38</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I40" s="2" t="e">
@@ -1564,16 +1507,13 @@
         <f t="shared" ref="K40" si="4">K41 - K39 - K38</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L40" s="2" t="e">
-        <f t="shared" ref="L40" si="5">L41 - L39 - L38</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="L40" s="2"/>
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="C41" s="2" t="e">
         <f>AVERAGE(Both[Newtonsoft])</f>
@@ -1604,17 +1544,14 @@
         <v>#DIV/0!</v>
       </c>
       <c r="J41" s="2" t="e">
-        <f>AVERAGE(Both[Boon])</f>
+        <f>AVERAGE(Both[Genson])</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K41" s="2" t="e">
-        <f>AVERAGE(Both[Alibaba])</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L41" s="2" t="e">
         <f>AVERAGE(Both[Gson])</f>
         <v>#DIV/0!</v>
       </c>
+      <c r="L41" s="2"/>
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
     </row>
@@ -1651,17 +1588,14 @@
         <v>#DIV/0!</v>
       </c>
       <c r="J42" s="2" t="e">
-        <f>AVERAGE(Serialization[Boon (size)])</f>
+        <f>AVERAGE(Serialization[Genson (size)])</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K42" s="2" t="e">
-        <f>AVERAGE(Serialization[Alibaba (size)])</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L42" s="2" t="e">
         <f>AVERAGE(Serialization[Gson (size)])</f>
         <v>#DIV/0!</v>
       </c>
+      <c r="L42" s="2"/>
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
     </row>
@@ -1679,34 +1613,31 @@
         <v>3</v>
       </c>
       <c r="C46" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D46" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E46" t="s">
         <v>12</v>
       </c>
       <c r="F46" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="G46" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="H46" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="I46" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J46" t="s">
-        <v>13</v>
+        <v>60</v>
       </c>
       <c r="K46" t="s">
-        <v>14</v>
-      </c>
-      <c r="L46" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="47" spans="2:14" x14ac:dyDescent="0.25">
@@ -1742,23 +1673,20 @@
         <v>#NUM!</v>
       </c>
       <c r="J47" s="2" t="e">
-        <f>DEVSQ(Serialization[Boon])</f>
+        <f>DEVSQ(Serialization[Genson])</f>
         <v>#NUM!</v>
       </c>
       <c r="K47" s="2" t="e">
-        <f>DEVSQ(Serialization[Alibaba])</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="L47" s="2" t="e">
         <f>DEVSQ(Serialization[Gson])</f>
         <v>#NUM!</v>
       </c>
+      <c r="L47" s="2"/>
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
     </row>
     <row r="48" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="C48" s="2" t="e">
         <f>DEVSQ(Both[Newtonsoft])</f>
@@ -1789,292 +1717,265 @@
         <v>#NUM!</v>
       </c>
       <c r="J48" s="2" t="e">
-        <f>DEVSQ(Both[Boon])</f>
+        <f>DEVSQ(Both[Genson])</f>
         <v>#NUM!</v>
       </c>
       <c r="K48" s="2" t="e">
-        <f>DEVSQ(Both[Alibaba])</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="L48" s="2" t="e">
         <f>DEVSQ(Both[Gson])</f>
         <v>#NUM!</v>
       </c>
+      <c r="L48" s="2"/>
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
     </row>
-    <row r="49" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
     </row>
-    <row r="50" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B50" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="51" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
-        <v>18</v>
-      </c>
       <c r="C51" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D51" t="s">
         <v>12</v>
       </c>
       <c r="E51" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="F51" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="G51" t="s">
         <v>6</v>
       </c>
       <c r="H51" t="s">
+        <v>18</v>
+      </c>
+      <c r="I51" t="s">
+        <v>60</v>
+      </c>
+      <c r="J51" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="52" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>19</v>
+      </c>
+      <c r="C52" t="s">
         <v>20</v>
       </c>
-      <c r="I51" t="s">
-        <v>13</v>
-      </c>
-      <c r="J51" t="s">
-        <v>14</v>
-      </c>
-      <c r="K51" t="s">
+      <c r="D52" t="s">
+        <v>21</v>
+      </c>
+      <c r="E52" t="s">
+        <v>22</v>
+      </c>
+      <c r="F52" t="s">
+        <v>24</v>
+      </c>
+      <c r="G52" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="52" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
-        <v>21</v>
-      </c>
-      <c r="C52" t="s">
-        <v>22</v>
-      </c>
-      <c r="D52" t="s">
-        <v>23</v>
-      </c>
-      <c r="E52" t="s">
-        <v>24</v>
-      </c>
-      <c r="F52" t="s">
+      <c r="H52" t="s">
         <v>26</v>
       </c>
-      <c r="G52" t="s">
+      <c r="I52" t="s">
+        <v>64</v>
+      </c>
+      <c r="J52" t="s">
         <v>27</v>
       </c>
-      <c r="H52" t="s">
-        <v>28</v>
-      </c>
-      <c r="I52" t="s">
-        <v>29</v>
-      </c>
-      <c r="J52" t="s">
-        <v>30</v>
-      </c>
-      <c r="K52" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="54" spans="2:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B54" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="55" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>16</v>
+      </c>
+      <c r="C55" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="55" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
-        <v>18</v>
-      </c>
-      <c r="C55" t="s">
-        <v>19</v>
       </c>
       <c r="D55" t="s">
         <v>12</v>
       </c>
       <c r="E55" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="F55" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="G55" t="s">
         <v>6</v>
       </c>
       <c r="H55" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I55" t="s">
-        <v>13</v>
+        <v>60</v>
       </c>
       <c r="J55" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="K55" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="L55" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="M55" t="s">
+        <v>41</v>
+      </c>
+      <c r="N55" t="s">
+        <v>43</v>
+      </c>
+      <c r="O55" t="s">
         <v>44</v>
       </c>
-      <c r="N55" t="s">
+      <c r="P55" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q55" t="s">
         <v>47</v>
       </c>
-      <c r="O55" t="s">
-        <v>49</v>
-      </c>
-      <c r="P55" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q55" t="s">
-        <v>7</v>
-      </c>
       <c r="R55" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="S55" t="s">
-        <v>57</v>
-      </c>
-      <c r="T55" t="s">
-        <v>63</v>
-      </c>
-      <c r="U55" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="56" spans="2:21" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="56" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C56" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D56" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E56" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="F56" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="G56" t="s">
         <v>8</v>
       </c>
       <c r="H56" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="I56" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="J56" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="K56" t="s">
+        <v>36</v>
+      </c>
+      <c r="L56" t="s">
+        <v>39</v>
+      </c>
+      <c r="M56" t="s">
+        <v>42</v>
+      </c>
+      <c r="N56" t="s">
+        <v>50</v>
+      </c>
+      <c r="O56" t="s">
+        <v>49</v>
+      </c>
+      <c r="P56" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q56" t="s">
+        <v>48</v>
+      </c>
+      <c r="R56" t="s">
+        <v>62</v>
+      </c>
+      <c r="S56" t="s">
         <v>54</v>
       </c>
-      <c r="L56" t="s">
-        <v>42</v>
-      </c>
-      <c r="M56" t="s">
-        <v>45</v>
-      </c>
-      <c r="N56" t="s">
-        <v>48</v>
-      </c>
-      <c r="O56" t="s">
-        <v>60</v>
-      </c>
-      <c r="P56" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q56" t="s">
-        <v>9</v>
-      </c>
-      <c r="R56" t="s">
-        <v>56</v>
-      </c>
-      <c r="S56" t="s">
-        <v>58</v>
-      </c>
-      <c r="T56" t="s">
-        <v>66</v>
-      </c>
-      <c r="U56" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="58" spans="2:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B58" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="59" spans="2:21" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="59" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C59" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D59" t="s">
         <v>12</v>
       </c>
       <c r="E59" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="F59" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="G59" t="s">
         <v>6</v>
       </c>
       <c r="H59" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I59" t="s">
-        <v>13</v>
+        <v>60</v>
       </c>
       <c r="J59" t="s">
-        <v>14</v>
-      </c>
-      <c r="K59" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="60" spans="2:21" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="60" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
+        <v>28</v>
+      </c>
+      <c r="C60" t="s">
+        <v>29</v>
+      </c>
+      <c r="D60" t="s">
+        <v>30</v>
+      </c>
+      <c r="E60" t="s">
+        <v>31</v>
+      </c>
+      <c r="F60" t="s">
         <v>32</v>
-      </c>
-      <c r="C60" t="s">
-        <v>33</v>
-      </c>
-      <c r="D60" t="s">
-        <v>34</v>
-      </c>
-      <c r="E60" t="s">
-        <v>35</v>
-      </c>
-      <c r="F60" t="s">
-        <v>36</v>
       </c>
       <c r="G60" t="s">
         <v>10</v>
       </c>
       <c r="H60" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="I60" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="J60" t="s">
-        <v>39</v>
-      </c>
-      <c r="K60" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed few more minor issues.
Redirect to NetJSON :D
Manual setup for NetJSON :(

Exclude type info in fastJSON

Show partially valid results during gathering.

TODO: rerun bench.
</commit_message>
<xml_diff>
--- a/GatherResults/template.xlsx
+++ b/GatherResults/template.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="84">
   <si>
     <t>Serialization</t>
   </si>
@@ -212,6 +212,60 @@
   </si>
   <si>
     <t>[[both.Genson.Duration]]</t>
+  </si>
+  <si>
+    <t>fastJSON</t>
+  </si>
+  <si>
+    <t>Alibaba</t>
+  </si>
+  <si>
+    <t>Boon</t>
+  </si>
+  <si>
+    <t>[[instance.fastJSON.Duration]]</t>
+  </si>
+  <si>
+    <t>[[serialization.fastJSON.Duration]]</t>
+  </si>
+  <si>
+    <t>[[both.fastJSON.Duration]]</t>
+  </si>
+  <si>
+    <t>fastJSON (size)</t>
+  </si>
+  <si>
+    <t>[[serialization.fastJSON.Size]]</t>
+  </si>
+  <si>
+    <t>[[serialization.Alibaba.Size]]</t>
+  </si>
+  <si>
+    <t>[[serialization.Boon.Size]]</t>
+  </si>
+  <si>
+    <t>[[instance.Boon.Duration]]</t>
+  </si>
+  <si>
+    <t>[[instance.Alibaba.Duration]]</t>
+  </si>
+  <si>
+    <t>[[serialization.Boon.Duration]]</t>
+  </si>
+  <si>
+    <t>[[serialization.Alibaba.Duration]]</t>
+  </si>
+  <si>
+    <t>[[both.Boon.Duration]]</t>
+  </si>
+  <si>
+    <t>[[both.Alibaba.Duration]]</t>
+  </si>
+  <si>
+    <t>Boon (size)</t>
+  </si>
+  <si>
+    <t>Alibaba (size)</t>
   </si>
 </sst>
 </file>
@@ -269,7 +323,25 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="24">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="#,##0.0"/>
     </dxf>
@@ -392,9 +464,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$C$37:$K$37</c:f>
+              <c:f>Sheet1!$C$37:$N$37</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>Newtonsoft</c:v>
                 </c:pt>
@@ -402,24 +474,33 @@
                   <c:v>Revenj</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>fastJSON</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Service Stack</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>Jil</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>NetJSON</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>Jackson afterburner</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>DSL Platform Java</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>Genson</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
+                  <c:v>Boon</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Alibaba</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>Gson</c:v>
                 </c:pt>
               </c:strCache>
@@ -427,10 +508,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$39:$K$39</c:f>
+              <c:f>Sheet1!$C$39:$N$39</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.0</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -456,6 +537,15 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -479,9 +569,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$C$37:$K$37</c:f>
+              <c:f>Sheet1!$C$37:$N$37</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>Newtonsoft</c:v>
                 </c:pt>
@@ -489,24 +579,33 @@
                   <c:v>Revenj</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>fastJSON</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Service Stack</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>Jil</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>NetJSON</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>Jackson afterburner</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>DSL Platform Java</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>Genson</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
+                  <c:v>Boon</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Alibaba</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>Gson</c:v>
                 </c:pt>
               </c:strCache>
@@ -514,10 +613,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$40:$K$40</c:f>
+              <c:f>Sheet1!$C$40:$N$40</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.0</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -543,6 +642,15 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -558,11 +666,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="114873856"/>
-        <c:axId val="114875392"/>
+        <c:axId val="94857088"/>
+        <c:axId val="94858624"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="114873856"/>
+        <c:axId val="94857088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -571,7 +679,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114875392"/>
+        <c:crossAx val="94858624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -579,7 +687,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="114875392"/>
+        <c:axId val="94858624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -610,7 +718,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114873856"/>
+        <c:crossAx val="94857088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -674,9 +782,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$C$37:$K$37</c:f>
+              <c:f>Sheet1!$C$37:$N$37</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>Newtonsoft</c:v>
                 </c:pt>
@@ -684,24 +792,33 @@
                   <c:v>Revenj</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>fastJSON</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Service Stack</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>Jil</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>NetJSON</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>Jackson afterburner</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>DSL Platform Java</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>Genson</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
+                  <c:v>Boon</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Alibaba</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>Gson</c:v>
                 </c:pt>
               </c:strCache>
@@ -709,10 +826,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$42:$K$42</c:f>
+              <c:f>Sheet1!$C$42:$N$42</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -722,7 +839,7 @@
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="#,##0.0">
+                <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="#,##0.0">
@@ -738,6 +855,15 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="#,##0.0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="#,##0.0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="#,##0.0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="#,##0.0">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -753,11 +879,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="114900352"/>
-        <c:axId val="114910336"/>
+        <c:axId val="97599488"/>
+        <c:axId val="97601024"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="114900352"/>
+        <c:axId val="97599488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -766,7 +892,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114910336"/>
+        <c:crossAx val="97601024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -774,7 +900,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="114910336"/>
+        <c:axId val="97601024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -805,7 +931,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114900352"/>
+        <c:crossAx val="97599488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -895,13 +1021,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Serialization" displayName="Serialization" ref="B55:S56">
-  <autoFilter ref="B55:S56"/>
-  <tableColumns count="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Serialization" displayName="Serialization" ref="B55:Y56">
+  <autoFilter ref="B55:Y56"/>
+  <tableColumns count="24">
     <tableColumn id="2" name="Newtonsoft" totalsRowFunction="custom">
       <totalsRowFormula>AverageNumbers[](Serialization[Newtonsoft])</totalsRowFormula>
     </tableColumn>
     <tableColumn id="7" name="Revenj"/>
+    <tableColumn id="10" name="fastJSON"/>
     <tableColumn id="1" name="Service Stack"/>
     <tableColumn id="3" name="Jil" totalsRowFunction="custom">
       <totalsRowFormula>AverageNumbers[](Serialization[Jil])</totalsRowFormula>
@@ -912,11 +1039,14 @@
       <totalsRowFormula>AverageNumbers[](Serialization[DSL Platform Java])</totalsRowFormula>
     </tableColumn>
     <tableColumn id="11" name="Genson"/>
+    <tableColumn id="24" name="Boon"/>
+    <tableColumn id="23" name="Alibaba"/>
     <tableColumn id="5" name="Gson" totalsRowFunction="custom">
       <totalsRowFormula>AverageNumbers[](Serialization[Gson])</totalsRowFormula>
     </tableColumn>
     <tableColumn id="15" name="Newtonsoft (size)"/>
     <tableColumn id="14" name="Revenj (size)"/>
+    <tableColumn id="19" name="fastJSON (size)"/>
     <tableColumn id="6" name="Service Stack (size)" totalsRowFunction="custom">
       <totalsRowFormula>AverageNumbers[](Serialization[Service Stack (size)])</totalsRowFormula>
     </tableColumn>
@@ -925,6 +1055,8 @@
     <tableColumn id="16" name="Jackson (size)"/>
     <tableColumn id="17" name="DSL Platform Java (size)"/>
     <tableColumn id="18" name="Genson (size)"/>
+    <tableColumn id="22" name="Boon (size)"/>
+    <tableColumn id="21" name="Alibaba (size)"/>
     <tableColumn id="20" name="Gson (size)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -932,45 +1064,51 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="AverageNumbers" displayName="AverageNumbers" ref="B37:K42" totalsRowShown="0">
-  <autoFilter ref="B37:K42"/>
-  <tableColumns count="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="AverageNumbers" displayName="AverageNumbers" ref="B37:N42" totalsRowShown="0">
+  <autoFilter ref="B37:N42"/>
+  <tableColumns count="13">
     <tableColumn id="1" name="Average"/>
-    <tableColumn id="2" name="Newtonsoft" dataDxfId="17">
+    <tableColumn id="2" name="Newtonsoft" dataDxfId="23">
       <calculatedColumnFormula>AverageNumbers[](Serialization[Newtonsoft])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Revenj" dataDxfId="16"/>
-    <tableColumn id="4" name="Service Stack" dataDxfId="15"/>
-    <tableColumn id="8" name="Jil" dataDxfId="14"/>
-    <tableColumn id="7" name="NetJSON" dataDxfId="13"/>
-    <tableColumn id="5" name="Jackson afterburner" dataDxfId="12"/>
-    <tableColumn id="6" name="DSL Platform Java" dataDxfId="11"/>
-    <tableColumn id="9" name="Genson" dataDxfId="10"/>
-    <tableColumn id="10" name="Gson" dataDxfId="1"/>
+    <tableColumn id="3" name="Revenj" dataDxfId="22"/>
+    <tableColumn id="11" name="fastJSON" dataDxfId="21"/>
+    <tableColumn id="4" name="Service Stack" dataDxfId="20"/>
+    <tableColumn id="8" name="Jil" dataDxfId="19"/>
+    <tableColumn id="7" name="NetJSON" dataDxfId="18"/>
+    <tableColumn id="5" name="Jackson afterburner" dataDxfId="17"/>
+    <tableColumn id="6" name="DSL Platform Java" dataDxfId="16"/>
+    <tableColumn id="9" name="Genson" dataDxfId="15"/>
+    <tableColumn id="13" name="Boon" dataDxfId="14"/>
+    <tableColumn id="12" name="Alibaba" dataDxfId="13"/>
+    <tableColumn id="10" name="Gson" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="DeviationNumbers" displayName="DeviationNumbers" ref="B46:K48" totalsRowShown="0">
-  <autoFilter ref="B46:K48"/>
-  <tableColumns count="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="DeviationNumbers" displayName="DeviationNumbers" ref="B46:N48" totalsRowShown="0">
+  <autoFilter ref="B46:N48"/>
+  <tableColumns count="13">
     <tableColumn id="1" name="Deviation"/>
-    <tableColumn id="2" name="Newtonsoft" dataDxfId="9">
+    <tableColumn id="2" name="Newtonsoft" dataDxfId="11">
       <calculatedColumnFormula>AverageNumbers[](Serialization[Newtonsoft])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Revenj" dataDxfId="8"/>
-    <tableColumn id="4" name="Service Stack" dataDxfId="7"/>
-    <tableColumn id="5" name="Jil" dataDxfId="6">
+    <tableColumn id="3" name="Revenj" dataDxfId="10"/>
+    <tableColumn id="11" name="fastJSON" dataDxfId="9"/>
+    <tableColumn id="4" name="Service Stack" dataDxfId="8"/>
+    <tableColumn id="5" name="Jil" dataDxfId="7">
       <calculatedColumnFormula>DEVSQ(Serialization[Jil])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="NetJSON" dataDxfId="5">
+    <tableColumn id="6" name="NetJSON" dataDxfId="6">
       <calculatedColumnFormula>DEVSQ(Both[NetJSON])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Jackson afterburner" dataDxfId="4"/>
-    <tableColumn id="8" name="DSL Platform Java" dataDxfId="3"/>
-    <tableColumn id="9" name="Genson" dataDxfId="2"/>
+    <tableColumn id="7" name="Jackson afterburner" dataDxfId="5"/>
+    <tableColumn id="8" name="DSL Platform Java" dataDxfId="4"/>
+    <tableColumn id="9" name="Genson" dataDxfId="3"/>
+    <tableColumn id="13" name="Boon" dataDxfId="2"/>
+    <tableColumn id="12" name="Alibaba" dataDxfId="1"/>
     <tableColumn id="10" name="Gson" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -978,13 +1116,14 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Both" displayName="Both" ref="B59:J60">
-  <autoFilter ref="B59:J60"/>
-  <tableColumns count="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Both" displayName="Both" ref="B59:M60">
+  <autoFilter ref="B59:M60"/>
+  <tableColumns count="12">
     <tableColumn id="2" name="Newtonsoft" totalsRowFunction="custom">
       <totalsRowFormula>AverageNumbers[](Both[Newtonsoft])</totalsRowFormula>
     </tableColumn>
     <tableColumn id="1" name="Revenj"/>
+    <tableColumn id="5" name="fastJSON"/>
     <tableColumn id="9" name="Service Stack"/>
     <tableColumn id="4" name="Jil" totalsRowFunction="custom">
       <totalsRowFormula>AverageNumbers[](Both[Jil])</totalsRowFormula>
@@ -995,6 +1134,8 @@
       <totalsRowFormula>AverageNumbers[](Both[DSL Platform Java])</totalsRowFormula>
     </tableColumn>
     <tableColumn id="3" name="Genson"/>
+    <tableColumn id="11" name="Boon"/>
+    <tableColumn id="8" name="Alibaba"/>
     <tableColumn id="7" name="Gson"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1002,13 +1143,14 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Instance" displayName="Instance" ref="B51:J52">
-  <autoFilter ref="B51:J52"/>
-  <tableColumns count="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Instance" displayName="Instance" ref="B51:M52">
+  <autoFilter ref="B51:M52"/>
+  <tableColumns count="12">
     <tableColumn id="2" name="Newtonsoft" totalsRowFunction="custom">
       <totalsRowFormula>AverageNumbers[](Instance[Newtonsoft])</totalsRowFormula>
     </tableColumn>
     <tableColumn id="1" name="Revenj"/>
+    <tableColumn id="5" name="fastJSON"/>
     <tableColumn id="9" name="Service Stack"/>
     <tableColumn id="4" name="Jil" totalsRowFunction="custom">
       <totalsRowFormula>AverageNumbers[](Instance[Jil])</totalsRowFormula>
@@ -1019,6 +1161,8 @@
       <totalsRowFormula>AverageNumbers[](Instance[DSL Platform Java])</totalsRowFormula>
     </tableColumn>
     <tableColumn id="3" name="Genson"/>
+    <tableColumn id="11" name="Boon"/>
+    <tableColumn id="8" name="Alibaba"/>
     <tableColumn id="7" name="Gson"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1312,10 +1456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:S60"/>
+  <dimension ref="B1:Y60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1334,10 +1478,11 @@
     <col min="13" max="13" width="25.85546875" customWidth="1"/>
     <col min="14" max="14" width="24.5703125" customWidth="1"/>
     <col min="15" max="15" width="22.140625" customWidth="1"/>
-    <col min="16" max="17" width="18.42578125" customWidth="1"/>
-    <col min="18" max="18" width="18.5703125" customWidth="1"/>
-    <col min="19" max="19" width="18.28515625" customWidth="1"/>
-    <col min="20" max="21" width="18.42578125" customWidth="1"/>
+    <col min="16" max="16" width="21.140625" customWidth="1"/>
+    <col min="17" max="17" width="21.42578125" customWidth="1"/>
+    <col min="18" max="18" width="21.5703125" customWidth="1"/>
+    <col min="19" max="20" width="21.7109375" customWidth="1"/>
+    <col min="21" max="21" width="21.5703125" customWidth="1"/>
     <col min="22" max="23" width="18.28515625" customWidth="1"/>
     <col min="24" max="24" width="18.7109375" customWidth="1"/>
   </cols>
@@ -1347,7 +1492,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>2</v>
       </c>
@@ -1358,28 +1503,37 @@
         <v>17</v>
       </c>
       <c r="E37" t="s">
+        <v>66</v>
+      </c>
+      <c r="F37" t="s">
         <v>12</v>
       </c>
-      <c r="F37" t="s">
+      <c r="G37" t="s">
         <v>56</v>
       </c>
-      <c r="G37" t="s">
+      <c r="H37" t="s">
         <v>55</v>
       </c>
-      <c r="H37" t="s">
+      <c r="I37" t="s">
         <v>59</v>
       </c>
-      <c r="I37" t="s">
+      <c r="J37" t="s">
         <v>18</v>
       </c>
-      <c r="J37" t="s">
+      <c r="K37" t="s">
         <v>60</v>
       </c>
-      <c r="K37" t="s">
+      <c r="L37" t="s">
+        <v>68</v>
+      </c>
+      <c r="M37" t="s">
+        <v>67</v>
+      </c>
+      <c r="N37" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>57</v>
       </c>
@@ -1392,38 +1546,50 @@
         <v>#DIV/0!</v>
       </c>
       <c r="E38" s="2" t="e">
+        <f>AVERAGE(Instance[fastJSON])</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F38" s="2" t="e">
         <f>AVERAGE(Instance[Service Stack])</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F38" s="2" t="e">
+      <c r="G38" s="2" t="e">
         <f>AVERAGE(Instance[Jil])</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G38" s="2" t="e">
+      <c r="H38" s="2" t="e">
         <f>AVERAGE(Instance[NetJSON])</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H38" s="2" t="e">
+      <c r="I38" s="2" t="e">
         <f>AVERAGE(Instance[Jackson])</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I38" s="2" t="e">
+      <c r="J38" s="2" t="e">
         <f>AVERAGE(Instance[DSL Platform Java])</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J38" s="2" t="e">
+      <c r="K38" s="2" t="e">
         <f>AVERAGE(Instance[Genson])</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K38" s="2" t="e">
+      <c r="L38" s="2" t="e">
+        <f>AVERAGE(Instance[Boon])</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M38" s="2" t="e">
+        <f>AVERAGE(Instance[Alibaba])</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N38" s="2" t="e">
         <f>AVERAGE(Instance[Gson])</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L38" s="2"/>
-      <c r="M38" s="2"/>
-      <c r="N38" s="2"/>
+      <c r="O38" s="2"/>
+      <c r="P38" s="2"/>
+      <c r="Q38" s="2"/>
     </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>0</v>
       </c>
@@ -1436,43 +1602,55 @@
         <v>#DIV/0!</v>
       </c>
       <c r="E39" s="2" t="e">
-        <f>AVERAGE(Serialization[Service Stack]) - E38</f>
+        <f>AVERAGE(Serialization[fastJSON]) - E38</f>
         <v>#DIV/0!</v>
       </c>
       <c r="F39" s="2" t="e">
-        <f>AVERAGE(Serialization[Jil]) - F38</f>
+        <f>AVERAGE(Serialization[Service Stack]) - F38</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G39" s="2" t="e">
-        <f>AVERAGE(Serialization[NetJSON]) - G38</f>
+        <f>AVERAGE(Serialization[Jil]) - G38</f>
         <v>#DIV/0!</v>
       </c>
       <c r="H39" s="2" t="e">
-        <f>AVERAGE(Serialization[Jackson]) - H38</f>
+        <f>AVERAGE(Serialization[NetJSON]) - H38</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I39" s="2" t="e">
-        <f>AVERAGE(Serialization[DSL Platform Java]) - I38</f>
+        <f>AVERAGE(Serialization[Jackson]) - I38</f>
         <v>#DIV/0!</v>
       </c>
       <c r="J39" s="2" t="e">
-        <f>AVERAGE(Serialization[Genson]) - J38</f>
+        <f>AVERAGE(Serialization[DSL Platform Java]) - J38</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K39" s="2" t="e">
-        <f>AVERAGE(Serialization[Gson]) - K38</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L39" s="2"/>
-      <c r="M39" s="2"/>
-      <c r="N39" s="2"/>
+        <f>AVERAGE(Serialization[Genson]) - K38</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L39" s="2" t="e">
+        <f>AVERAGE(Serialization[Boon]) - L38</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M39" s="2" t="e">
+        <f>AVERAGE(Serialization[Alibaba]) - M38</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N39" s="2" t="e">
+        <f>AVERAGE(Serialization[Gson]) - N38</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O39" s="2"/>
+      <c r="P39" s="2"/>
+      <c r="Q39" s="2"/>
     </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>1</v>
       </c>
       <c r="C40" s="2" t="e">
-        <f t="shared" ref="C40:G40" si="0">C41 - C39 - C38</f>
+        <f t="shared" ref="C40:H40" si="0">C41 - C39 - C38</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D40" s="2" t="e">
@@ -1480,7 +1658,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="E40" s="2" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="E40" si="1">E41 - E39 - E38</f>
         <v>#DIV/0!</v>
       </c>
       <c r="F40" s="2" t="e">
@@ -1492,7 +1670,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="H40" s="2" t="e">
-        <f t="shared" ref="H40" si="1">H41 - H39 - H38</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I40" s="2" t="e">
@@ -1504,14 +1682,26 @@
         <v>#DIV/0!</v>
       </c>
       <c r="K40" s="2" t="e">
-        <f t="shared" ref="K40" si="4">K41 - K39 - K38</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L40" s="2"/>
-      <c r="M40" s="2"/>
-      <c r="N40" s="2"/>
+        <f t="shared" ref="K40:L40" si="4">K41 - K39 - K38</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L40" s="2" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M40" s="2" t="e">
+        <f t="shared" ref="M40" si="5">M41 - M39 - M38</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N40" s="2" t="e">
+        <f t="shared" ref="N40" si="6">N41 - N39 - N38</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O40" s="2"/>
+      <c r="P40" s="2"/>
+      <c r="Q40" s="2"/>
     </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>58</v>
       </c>
@@ -1524,38 +1714,50 @@
         <v>#DIV/0!</v>
       </c>
       <c r="E41" s="2" t="e">
+        <f>AVERAGE(Both[fastJSON])</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F41" s="2" t="e">
         <f>AVERAGE(Both[Service Stack])</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F41" s="2" t="e">
+      <c r="G41" s="2" t="e">
         <f>AVERAGE(Both[Jil])</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G41" s="2" t="e">
+      <c r="H41" s="2" t="e">
         <f>AVERAGE(Both[NetJSON])</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H41" s="2" t="e">
+      <c r="I41" s="2" t="e">
         <f>AVERAGE(Both[Jackson])</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I41" s="2" t="e">
+      <c r="J41" s="2" t="e">
         <f>AVERAGE(Both[DSL Platform Java])</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J41" s="2" t="e">
+      <c r="K41" s="2" t="e">
         <f>AVERAGE(Both[Genson])</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K41" s="2" t="e">
+      <c r="L41" s="2" t="e">
+        <f>AVERAGE(Both[Boon])</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M41" s="2" t="e">
+        <f>AVERAGE(Both[Alibaba])</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N41" s="2" t="e">
         <f>AVERAGE(Both[Gson])</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L41" s="2"/>
-      <c r="M41" s="2"/>
-      <c r="N41" s="2"/>
+      <c r="O41" s="2"/>
+      <c r="P41" s="2"/>
+      <c r="Q41" s="2"/>
     </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>4</v>
       </c>
@@ -1568,38 +1770,50 @@
         <v>#DIV/0!</v>
       </c>
       <c r="E42" s="3" t="e">
+        <f>AVERAGE(Serialization[fastJSON (size)])</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F42" s="3" t="e">
         <f>AVERAGE(Serialization[Service Stack (size)])</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F42" s="2" t="e">
+      <c r="G42" s="2" t="e">
         <f>AVERAGE(Serialization[Jil (size)])</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G42" s="2" t="e">
+      <c r="H42" s="2" t="e">
         <f>AVERAGE(Serialization[NetJSON (size)])</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H42" s="2" t="e">
+      <c r="I42" s="2" t="e">
         <f>AVERAGE(Serialization[Jackson (size)])</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I42" s="2" t="e">
+      <c r="J42" s="2" t="e">
         <f>AVERAGE(Serialization[DSL Platform Java (size)])</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J42" s="2" t="e">
+      <c r="K42" s="2" t="e">
         <f>AVERAGE(Serialization[Genson (size)])</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K42" s="2" t="e">
+      <c r="L42" s="2" t="e">
+        <f>AVERAGE(Serialization[Boon (size)])</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M42" s="2" t="e">
+        <f>AVERAGE(Serialization[Alibaba (size)])</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N42" s="2" t="e">
         <f>AVERAGE(Serialization[Gson (size)])</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L42" s="2"/>
-      <c r="M42" s="2"/>
-      <c r="N42" s="2"/>
+      <c r="O42" s="2"/>
+      <c r="P42" s="2"/>
+      <c r="Q42" s="2"/>
     </row>
-    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
@@ -1608,7 +1822,7 @@
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
     </row>
-    <row r="46" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>3</v>
       </c>
@@ -1619,28 +1833,37 @@
         <v>17</v>
       </c>
       <c r="E46" t="s">
+        <v>66</v>
+      </c>
+      <c r="F46" t="s">
         <v>12</v>
       </c>
-      <c r="F46" t="s">
+      <c r="G46" t="s">
         <v>56</v>
       </c>
-      <c r="G46" t="s">
+      <c r="H46" t="s">
         <v>55</v>
       </c>
-      <c r="H46" t="s">
+      <c r="I46" t="s">
         <v>59</v>
       </c>
-      <c r="I46" t="s">
+      <c r="J46" t="s">
         <v>18</v>
       </c>
-      <c r="J46" t="s">
+      <c r="K46" t="s">
         <v>60</v>
       </c>
-      <c r="K46" t="s">
+      <c r="L46" t="s">
+        <v>68</v>
+      </c>
+      <c r="M46" t="s">
+        <v>67</v>
+      </c>
+      <c r="N46" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="47" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>0</v>
       </c>
@@ -1653,38 +1876,50 @@
         <v>#NUM!</v>
       </c>
       <c r="E47" s="2" t="e">
+        <f>DEVSQ(Serialization[fastJSON])</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="F47" s="2" t="e">
         <f>DEVSQ(Serialization[Service Stack])</f>
         <v>#NUM!</v>
       </c>
-      <c r="F47" s="2" t="e">
+      <c r="G47" s="2" t="e">
         <f>DEVSQ(Serialization[Jil])</f>
         <v>#NUM!</v>
       </c>
-      <c r="G47" s="2" t="e">
+      <c r="H47" s="2" t="e">
         <f>DEVSQ(Serialization[NetJSON])</f>
         <v>#NUM!</v>
       </c>
-      <c r="H47" s="2" t="e">
+      <c r="I47" s="2" t="e">
         <f>DEVSQ(Serialization[Jackson])</f>
         <v>#NUM!</v>
       </c>
-      <c r="I47" s="2" t="e">
+      <c r="J47" s="2" t="e">
         <f>DEVSQ(Serialization[DSL Platform Java])</f>
         <v>#NUM!</v>
       </c>
-      <c r="J47" s="2" t="e">
+      <c r="K47" s="2" t="e">
         <f>DEVSQ(Serialization[Genson])</f>
         <v>#NUM!</v>
       </c>
-      <c r="K47" s="2" t="e">
+      <c r="L47" s="2" t="e">
+        <f>DEVSQ(Serialization[Boon])</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="M47" s="2" t="e">
+        <f>DEVSQ(Serialization[Alibaba])</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="N47" s="2" t="e">
         <f>DEVSQ(Serialization[Gson])</f>
         <v>#NUM!</v>
       </c>
-      <c r="L47" s="2"/>
-      <c r="M47" s="2"/>
-      <c r="N47" s="2"/>
+      <c r="O47" s="2"/>
+      <c r="P47" s="2"/>
+      <c r="Q47" s="2"/>
     </row>
-    <row r="48" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>58</v>
       </c>
@@ -1697,50 +1932,62 @@
         <v>#NUM!</v>
       </c>
       <c r="E48" s="2" t="e">
+        <f>DEVSQ(Both[fastJSON])</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="F48" s="2" t="e">
         <f>DEVSQ(Both[Service Stack])</f>
         <v>#NUM!</v>
       </c>
-      <c r="F48" s="2" t="e">
+      <c r="G48" s="2" t="e">
         <f>DEVSQ(Both[Jil])</f>
         <v>#NUM!</v>
       </c>
-      <c r="G48" s="2" t="e">
+      <c r="H48" s="2" t="e">
         <f>DEVSQ(Both[NetJSON])</f>
         <v>#NUM!</v>
       </c>
-      <c r="H48" s="2" t="e">
+      <c r="I48" s="2" t="e">
         <f>DEVSQ(Both[Jackson])</f>
         <v>#NUM!</v>
       </c>
-      <c r="I48" s="2" t="e">
+      <c r="J48" s="2" t="e">
         <f>DEVSQ(Both[DSL Platform Java])</f>
         <v>#NUM!</v>
       </c>
-      <c r="J48" s="2" t="e">
+      <c r="K48" s="2" t="e">
         <f>DEVSQ(Both[Genson])</f>
         <v>#NUM!</v>
       </c>
-      <c r="K48" s="2" t="e">
+      <c r="L48" s="2" t="e">
+        <f>DEVSQ(Both[Boon])</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="M48" s="2" t="e">
+        <f>DEVSQ(Both[Alibaba])</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="N48" s="2" t="e">
         <f>DEVSQ(Both[Gson])</f>
         <v>#NUM!</v>
       </c>
-      <c r="L48" s="2"/>
-      <c r="M48" s="2"/>
-      <c r="N48" s="2"/>
+      <c r="O48" s="2"/>
+      <c r="P48" s="2"/>
+      <c r="Q48" s="2"/>
     </row>
-    <row r="49" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:25" x14ac:dyDescent="0.25">
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
     </row>
-    <row r="50" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B50" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="51" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>16</v>
       </c>
@@ -1748,28 +1995,37 @@
         <v>17</v>
       </c>
       <c r="D51" t="s">
+        <v>66</v>
+      </c>
+      <c r="E51" t="s">
         <v>12</v>
       </c>
-      <c r="E51" t="s">
+      <c r="F51" t="s">
         <v>56</v>
       </c>
-      <c r="F51" t="s">
+      <c r="G51" t="s">
         <v>55</v>
       </c>
-      <c r="G51" t="s">
+      <c r="H51" t="s">
         <v>6</v>
       </c>
-      <c r="H51" t="s">
+      <c r="I51" t="s">
         <v>18</v>
       </c>
-      <c r="I51" t="s">
+      <c r="J51" t="s">
         <v>60</v>
       </c>
-      <c r="J51" t="s">
+      <c r="K51" t="s">
+        <v>68</v>
+      </c>
+      <c r="L51" t="s">
+        <v>67</v>
+      </c>
+      <c r="M51" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="52" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>19</v>
       </c>
@@ -1777,33 +2033,42 @@
         <v>20</v>
       </c>
       <c r="D52" t="s">
+        <v>69</v>
+      </c>
+      <c r="E52" t="s">
         <v>21</v>
       </c>
-      <c r="E52" t="s">
+      <c r="F52" t="s">
         <v>22</v>
       </c>
-      <c r="F52" t="s">
+      <c r="G52" t="s">
         <v>24</v>
       </c>
-      <c r="G52" t="s">
+      <c r="H52" t="s">
         <v>25</v>
       </c>
-      <c r="H52" t="s">
+      <c r="I52" t="s">
         <v>26</v>
       </c>
-      <c r="I52" t="s">
+      <c r="J52" t="s">
         <v>64</v>
       </c>
-      <c r="J52" t="s">
+      <c r="K52" t="s">
+        <v>76</v>
+      </c>
+      <c r="L52" t="s">
+        <v>77</v>
+      </c>
+      <c r="M52" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B54" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>16</v>
       </c>
@@ -1811,55 +2076,73 @@
         <v>17</v>
       </c>
       <c r="D55" t="s">
+        <v>66</v>
+      </c>
+      <c r="E55" t="s">
         <v>12</v>
       </c>
-      <c r="E55" t="s">
+      <c r="F55" t="s">
         <v>56</v>
       </c>
-      <c r="F55" t="s">
+      <c r="G55" t="s">
         <v>55</v>
       </c>
-      <c r="G55" t="s">
+      <c r="H55" t="s">
         <v>6</v>
       </c>
-      <c r="H55" t="s">
+      <c r="I55" t="s">
         <v>18</v>
       </c>
-      <c r="I55" t="s">
+      <c r="J55" t="s">
         <v>60</v>
       </c>
-      <c r="J55" t="s">
+      <c r="K55" t="s">
+        <v>68</v>
+      </c>
+      <c r="L55" t="s">
+        <v>67</v>
+      </c>
+      <c r="M55" t="s">
         <v>23</v>
       </c>
-      <c r="K55" t="s">
+      <c r="N55" t="s">
         <v>5</v>
       </c>
-      <c r="L55" t="s">
+      <c r="O55" t="s">
         <v>38</v>
       </c>
-      <c r="M55" t="s">
+      <c r="P55" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q55" t="s">
         <v>41</v>
       </c>
-      <c r="N55" t="s">
+      <c r="R55" t="s">
         <v>43</v>
       </c>
-      <c r="O55" t="s">
+      <c r="S55" t="s">
         <v>44</v>
       </c>
-      <c r="P55" t="s">
+      <c r="T55" t="s">
         <v>7</v>
       </c>
-      <c r="Q55" t="s">
+      <c r="U55" t="s">
         <v>47</v>
       </c>
-      <c r="R55" t="s">
+      <c r="V55" t="s">
         <v>61</v>
       </c>
-      <c r="S55" t="s">
+      <c r="W55" t="s">
+        <v>82</v>
+      </c>
+      <c r="X55" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y55" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>35</v>
       </c>
@@ -1867,60 +2150,78 @@
         <v>37</v>
       </c>
       <c r="D56" t="s">
+        <v>70</v>
+      </c>
+      <c r="E56" t="s">
         <v>40</v>
       </c>
-      <c r="E56" t="s">
+      <c r="F56" t="s">
         <v>52</v>
       </c>
-      <c r="F56" t="s">
+      <c r="G56" t="s">
         <v>51</v>
       </c>
-      <c r="G56" t="s">
+      <c r="H56" t="s">
         <v>8</v>
       </c>
-      <c r="H56" t="s">
+      <c r="I56" t="s">
         <v>45</v>
       </c>
-      <c r="I56" t="s">
+      <c r="J56" t="s">
         <v>63</v>
       </c>
-      <c r="J56" t="s">
+      <c r="K56" t="s">
+        <v>78</v>
+      </c>
+      <c r="L56" t="s">
+        <v>79</v>
+      </c>
+      <c r="M56" t="s">
         <v>46</v>
       </c>
-      <c r="K56" t="s">
+      <c r="N56" t="s">
         <v>36</v>
       </c>
-      <c r="L56" t="s">
+      <c r="O56" t="s">
         <v>39</v>
       </c>
-      <c r="M56" t="s">
+      <c r="P56" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q56" t="s">
         <v>42</v>
       </c>
-      <c r="N56" t="s">
+      <c r="R56" t="s">
         <v>50</v>
       </c>
-      <c r="O56" t="s">
+      <c r="S56" t="s">
         <v>49</v>
       </c>
-      <c r="P56" t="s">
+      <c r="T56" t="s">
         <v>9</v>
       </c>
-      <c r="Q56" t="s">
+      <c r="U56" t="s">
         <v>48</v>
       </c>
-      <c r="R56" t="s">
+      <c r="V56" t="s">
         <v>62</v>
       </c>
-      <c r="S56" t="s">
+      <c r="W56" t="s">
+        <v>75</v>
+      </c>
+      <c r="X56" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y56" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="58" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B58" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="59" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>16</v>
       </c>
@@ -1928,28 +2229,37 @@
         <v>17</v>
       </c>
       <c r="D59" t="s">
+        <v>66</v>
+      </c>
+      <c r="E59" t="s">
         <v>12</v>
       </c>
-      <c r="E59" t="s">
+      <c r="F59" t="s">
         <v>56</v>
       </c>
-      <c r="F59" t="s">
+      <c r="G59" t="s">
         <v>55</v>
       </c>
-      <c r="G59" t="s">
+      <c r="H59" t="s">
         <v>6</v>
       </c>
-      <c r="H59" t="s">
+      <c r="I59" t="s">
         <v>18</v>
       </c>
-      <c r="I59" t="s">
+      <c r="J59" t="s">
         <v>60</v>
       </c>
-      <c r="J59" t="s">
+      <c r="K59" t="s">
+        <v>68</v>
+      </c>
+      <c r="L59" t="s">
+        <v>67</v>
+      </c>
+      <c r="M59" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="60" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>28</v>
       </c>
@@ -1957,24 +2267,33 @@
         <v>29</v>
       </c>
       <c r="D60" t="s">
+        <v>71</v>
+      </c>
+      <c r="E60" t="s">
         <v>30</v>
       </c>
-      <c r="E60" t="s">
+      <c r="F60" t="s">
         <v>31</v>
       </c>
-      <c r="F60" t="s">
+      <c r="G60" t="s">
         <v>32</v>
       </c>
-      <c r="G60" t="s">
+      <c r="H60" t="s">
         <v>10</v>
       </c>
-      <c r="H60" t="s">
+      <c r="I60" t="s">
         <v>33</v>
       </c>
-      <c r="I60" t="s">
+      <c r="J60" t="s">
         <v>65</v>
       </c>
-      <c r="J60" t="s">
+      <c r="K60" t="s">
+        <v>80</v>
+      </c>
+      <c r="L60" t="s">
+        <v>81</v>
+      </c>
+      <c r="M60" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updating dependencies to latest.
Switching from DslClientJava to DslJson

Switched fastJSON and Genson with binary counterparts for referenca values.

Genson can't deserialize anything and while fastJSON works ok, Jil and NetJSON are more popular.

TODO: rerun the bench
</commit_message>
<xml_diff>
--- a/GatherResults/template.xlsx
+++ b/GatherResults/template.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="85">
   <si>
     <t>Serialization</t>
   </si>
@@ -70,9 +70,6 @@
     <t>Revenj</t>
   </si>
   <si>
-    <t>DSL Platform Java</t>
-  </si>
-  <si>
     <t>[[instance.Newtonsoft.Duration]]</t>
   </si>
   <si>
@@ -94,9 +91,6 @@
     <t>[[instance.Jackson.Duration]]</t>
   </si>
   <si>
-    <t>[[instance.DslJava.Duration]]</t>
-  </si>
-  <si>
     <t>[[instance.Gson.Duration]]</t>
   </si>
   <si>
@@ -115,9 +109,6 @@
     <t>[[both.NetJSON.Duration]]</t>
   </si>
   <si>
-    <t>[[both.DslJava.Duration]]</t>
-  </si>
-  <si>
     <t>[[both.Gson.Duration]]</t>
   </si>
   <si>
@@ -151,15 +142,9 @@
     <t>NetJSON (size)</t>
   </si>
   <si>
-    <t>[[serialization.DslJava.Duration]]</t>
-  </si>
-  <si>
     <t>[[serialization.Gson.Duration]]</t>
   </si>
   <si>
-    <t>DSL Platform Java (size)</t>
-  </si>
-  <si>
     <t>[[serialization.DslJava.Size]]</t>
   </si>
   <si>
@@ -196,48 +181,12 @@
     <t>Jackson afterburner</t>
   </si>
   <si>
-    <t>Genson</t>
-  </si>
-  <si>
-    <t>Genson (size)</t>
-  </si>
-  <si>
-    <t>[[serialization.Genson.Size]]</t>
-  </si>
-  <si>
-    <t>[[serialization.Genson.Duration]]</t>
-  </si>
-  <si>
-    <t>[[instance.Genson.Duration]]</t>
-  </si>
-  <si>
-    <t>[[both.Genson.Duration]]</t>
-  </si>
-  <si>
-    <t>fastJSON</t>
-  </si>
-  <si>
     <t>Alibaba</t>
   </si>
   <si>
     <t>Boon</t>
   </si>
   <si>
-    <t>[[instance.fastJSON.Duration]]</t>
-  </si>
-  <si>
-    <t>[[serialization.fastJSON.Duration]]</t>
-  </si>
-  <si>
-    <t>[[both.fastJSON.Duration]]</t>
-  </si>
-  <si>
-    <t>fastJSON (size)</t>
-  </si>
-  <si>
-    <t>[[serialization.fastJSON.Size]]</t>
-  </si>
-  <si>
     <t>[[serialization.Alibaba.Size]]</t>
   </si>
   <si>
@@ -266,6 +215,60 @@
   </si>
   <si>
     <t>Alibaba (size)</t>
+  </si>
+  <si>
+    <t>DSL-JSON</t>
+  </si>
+  <si>
+    <t>[[instance.DslJson.Duration]]</t>
+  </si>
+  <si>
+    <t>[[serialization.DslJson.Duration]]</t>
+  </si>
+  <si>
+    <t>[[both.DslJson.Duration]]</t>
+  </si>
+  <si>
+    <t>DSL-JSON (size)</t>
+  </si>
+  <si>
+    <t>ProtoBuf (binary reference)</t>
+  </si>
+  <si>
+    <t>Protobuf (binary reference)</t>
+  </si>
+  <si>
+    <t>Kryo (binary reference)</t>
+  </si>
+  <si>
+    <t>ProtoBuf (size)</t>
+  </si>
+  <si>
+    <t>Kryo (size)</t>
+  </si>
+  <si>
+    <t>[[serialization.Kryo.Size]]</t>
+  </si>
+  <si>
+    <t>[[serialization.Protobuf.Size]]</t>
+  </si>
+  <si>
+    <t>[[serialization.Kryo.Duration]]</t>
+  </si>
+  <si>
+    <t>[[serialization.Protobuf.Duration]]</t>
+  </si>
+  <si>
+    <t>[[instance.Protobuf.Duration]]</t>
+  </si>
+  <si>
+    <t>[[instance.Kryo.Duration]]</t>
+  </si>
+  <si>
+    <t>[[both.Kryo.Duration]]</t>
+  </si>
+  <si>
+    <t>[[both.Protobuf.Duration]]</t>
   </si>
 </sst>
 </file>
@@ -474,7 +477,7 @@
                   <c:v>Revenj</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>fastJSON</c:v>
+                  <c:v>ProtoBuf (binary reference)</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Service Stack</c:v>
@@ -489,10 +492,10 @@
                   <c:v>Jackson afterburner</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>DSL Platform Java</c:v>
+                  <c:v>DSL-JSON</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Genson</c:v>
+                  <c:v>Kryo (binary reference)</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>Boon</c:v>
@@ -579,7 +582,7 @@
                   <c:v>Revenj</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>fastJSON</c:v>
+                  <c:v>ProtoBuf (binary reference)</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Service Stack</c:v>
@@ -594,10 +597,10 @@
                   <c:v>Jackson afterburner</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>DSL Platform Java</c:v>
+                  <c:v>DSL-JSON</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Genson</c:v>
+                  <c:v>Kryo (binary reference)</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>Boon</c:v>
@@ -666,11 +669,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="94857088"/>
-        <c:axId val="94858624"/>
+        <c:axId val="105637760"/>
+        <c:axId val="105639296"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="94857088"/>
+        <c:axId val="105637760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -679,7 +682,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94858624"/>
+        <c:crossAx val="105639296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -687,7 +690,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="94858624"/>
+        <c:axId val="105639296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -718,7 +721,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94857088"/>
+        <c:crossAx val="105637760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -792,7 +795,7 @@
                   <c:v>Revenj</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>fastJSON</c:v>
+                  <c:v>ProtoBuf (binary reference)</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Service Stack</c:v>
@@ -807,10 +810,10 @@
                   <c:v>Jackson afterburner</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>DSL Platform Java</c:v>
+                  <c:v>DSL-JSON</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Genson</c:v>
+                  <c:v>Kryo (binary reference)</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>Boon</c:v>
@@ -879,11 +882,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="97599488"/>
-        <c:axId val="97601024"/>
+        <c:axId val="106213376"/>
+        <c:axId val="106214912"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="97599488"/>
+        <c:axId val="106213376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -892,7 +895,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97601024"/>
+        <c:crossAx val="106214912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -900,7 +903,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="97601024"/>
+        <c:axId val="106214912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -931,7 +934,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97599488"/>
+        <c:crossAx val="106213376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1028,17 +1031,17 @@
       <totalsRowFormula>AverageNumbers[](Serialization[Newtonsoft])</totalsRowFormula>
     </tableColumn>
     <tableColumn id="7" name="Revenj"/>
-    <tableColumn id="10" name="fastJSON"/>
+    <tableColumn id="10" name="ProtoBuf (binary reference)"/>
     <tableColumn id="1" name="Service Stack"/>
     <tableColumn id="3" name="Jil" totalsRowFunction="custom">
       <totalsRowFormula>AverageNumbers[](Serialization[Jil])</totalsRowFormula>
     </tableColumn>
     <tableColumn id="9" name="NetJSON"/>
     <tableColumn id="8" name="Jackson"/>
-    <tableColumn id="4" name="DSL Platform Java" totalsRowFunction="custom">
-      <totalsRowFormula>AverageNumbers[](Serialization[DSL Platform Java])</totalsRowFormula>
+    <tableColumn id="4" name="DSL-JSON" totalsRowFunction="custom">
+      <totalsRowFormula>AverageNumbers[](Serialization[DSL-JSON])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="11" name="Genson"/>
+    <tableColumn id="11" name="Kryo (binary reference)"/>
     <tableColumn id="24" name="Boon"/>
     <tableColumn id="23" name="Alibaba"/>
     <tableColumn id="5" name="Gson" totalsRowFunction="custom">
@@ -1046,15 +1049,15 @@
     </tableColumn>
     <tableColumn id="15" name="Newtonsoft (size)"/>
     <tableColumn id="14" name="Revenj (size)"/>
-    <tableColumn id="19" name="fastJSON (size)"/>
+    <tableColumn id="19" name="ProtoBuf (size)"/>
     <tableColumn id="6" name="Service Stack (size)" totalsRowFunction="custom">
       <totalsRowFormula>AverageNumbers[](Serialization[Service Stack (size)])</totalsRowFormula>
     </tableColumn>
     <tableColumn id="13" name="Jil (size)"/>
     <tableColumn id="12" name="NetJSON (size)"/>
     <tableColumn id="16" name="Jackson (size)"/>
-    <tableColumn id="17" name="DSL Platform Java (size)"/>
-    <tableColumn id="18" name="Genson (size)"/>
+    <tableColumn id="17" name="DSL-JSON (size)"/>
+    <tableColumn id="18" name="Kryo (size)"/>
     <tableColumn id="22" name="Boon (size)"/>
     <tableColumn id="21" name="Alibaba (size)"/>
     <tableColumn id="20" name="Gson (size)"/>
@@ -1072,13 +1075,13 @@
       <calculatedColumnFormula>AverageNumbers[](Serialization[Newtonsoft])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" name="Revenj" dataDxfId="22"/>
-    <tableColumn id="11" name="fastJSON" dataDxfId="21"/>
+    <tableColumn id="11" name="ProtoBuf (binary reference)" dataDxfId="21"/>
     <tableColumn id="4" name="Service Stack" dataDxfId="20"/>
     <tableColumn id="8" name="Jil" dataDxfId="19"/>
     <tableColumn id="7" name="NetJSON" dataDxfId="18"/>
     <tableColumn id="5" name="Jackson afterburner" dataDxfId="17"/>
-    <tableColumn id="6" name="DSL Platform Java" dataDxfId="16"/>
-    <tableColumn id="9" name="Genson" dataDxfId="15"/>
+    <tableColumn id="6" name="DSL-JSON" dataDxfId="16"/>
+    <tableColumn id="9" name="Kryo (binary reference)" dataDxfId="15"/>
     <tableColumn id="13" name="Boon" dataDxfId="14"/>
     <tableColumn id="12" name="Alibaba" dataDxfId="13"/>
     <tableColumn id="10" name="Gson" dataDxfId="12"/>
@@ -1096,7 +1099,7 @@
       <calculatedColumnFormula>AverageNumbers[](Serialization[Newtonsoft])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" name="Revenj" dataDxfId="10"/>
-    <tableColumn id="11" name="fastJSON" dataDxfId="9"/>
+    <tableColumn id="11" name="Protobuf (binary reference)" dataDxfId="9"/>
     <tableColumn id="4" name="Service Stack" dataDxfId="8"/>
     <tableColumn id="5" name="Jil" dataDxfId="7">
       <calculatedColumnFormula>DEVSQ(Serialization[Jil])</calculatedColumnFormula>
@@ -1105,8 +1108,8 @@
       <calculatedColumnFormula>DEVSQ(Both[NetJSON])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" name="Jackson afterburner" dataDxfId="5"/>
-    <tableColumn id="8" name="DSL Platform Java" dataDxfId="4"/>
-    <tableColumn id="9" name="Genson" dataDxfId="3"/>
+    <tableColumn id="8" name="DSL-JSON" dataDxfId="4"/>
+    <tableColumn id="9" name="Kryo (binary reference)" dataDxfId="3"/>
     <tableColumn id="13" name="Boon" dataDxfId="2"/>
     <tableColumn id="12" name="Alibaba" dataDxfId="1"/>
     <tableColumn id="10" name="Gson" dataDxfId="0"/>
@@ -1123,17 +1126,17 @@
       <totalsRowFormula>AverageNumbers[](Both[Newtonsoft])</totalsRowFormula>
     </tableColumn>
     <tableColumn id="1" name="Revenj"/>
-    <tableColumn id="5" name="fastJSON"/>
+    <tableColumn id="5" name="ProtoBuf (binary reference)"/>
     <tableColumn id="9" name="Service Stack"/>
     <tableColumn id="4" name="Jil" totalsRowFunction="custom">
       <totalsRowFormula>AverageNumbers[](Both[Jil])</totalsRowFormula>
     </tableColumn>
     <tableColumn id="10" name="NetJSON"/>
     <tableColumn id="15" name="Jackson"/>
-    <tableColumn id="6" name="DSL Platform Java" totalsRowFunction="custom">
-      <totalsRowFormula>AverageNumbers[](Both[DSL Platform Java])</totalsRowFormula>
+    <tableColumn id="6" name="DSL-JSON" totalsRowFunction="custom">
+      <totalsRowFormula>AverageNumbers[](Both[DSL-JSON])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" name="Genson"/>
+    <tableColumn id="3" name="Kryo (binary reference)"/>
     <tableColumn id="11" name="Boon"/>
     <tableColumn id="8" name="Alibaba"/>
     <tableColumn id="7" name="Gson"/>
@@ -1150,17 +1153,17 @@
       <totalsRowFormula>AverageNumbers[](Instance[Newtonsoft])</totalsRowFormula>
     </tableColumn>
     <tableColumn id="1" name="Revenj"/>
-    <tableColumn id="5" name="fastJSON"/>
+    <tableColumn id="5" name="ProtoBuf (binary reference)"/>
     <tableColumn id="9" name="Service Stack"/>
     <tableColumn id="4" name="Jil" totalsRowFunction="custom">
       <totalsRowFormula>AverageNumbers[](Instance[Jil])</totalsRowFormula>
     </tableColumn>
     <tableColumn id="10" name="NetJSON"/>
     <tableColumn id="15" name="Jackson"/>
-    <tableColumn id="6" name="DSL Platform Java" totalsRowFunction="custom">
-      <totalsRowFormula>AverageNumbers[](Instance[DSL Platform Java])</totalsRowFormula>
+    <tableColumn id="6" name="DSL-JSON" totalsRowFunction="custom">
+      <totalsRowFormula>AverageNumbers[](Instance[DSL-JSON])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" name="Genson"/>
+    <tableColumn id="3" name="Kryo (binary reference)"/>
     <tableColumn id="11" name="Boon"/>
     <tableColumn id="8" name="Alibaba"/>
     <tableColumn id="7" name="Gson"/>
@@ -1458,9 +1461,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Y60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1485,6 +1486,7 @@
     <col min="21" max="21" width="21.5703125" customWidth="1"/>
     <col min="22" max="23" width="18.28515625" customWidth="1"/>
     <col min="24" max="24" width="18.7109375" customWidth="1"/>
+    <col min="25" max="25" width="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:2" x14ac:dyDescent="0.25">
@@ -1503,39 +1505,39 @@
         <v>17</v>
       </c>
       <c r="E37" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F37" t="s">
         <v>12</v>
       </c>
       <c r="G37" t="s">
+        <v>51</v>
+      </c>
+      <c r="H37" t="s">
+        <v>50</v>
+      </c>
+      <c r="I37" t="s">
+        <v>54</v>
+      </c>
+      <c r="J37" t="s">
+        <v>67</v>
+      </c>
+      <c r="K37" t="s">
+        <v>74</v>
+      </c>
+      <c r="L37" t="s">
         <v>56</v>
       </c>
-      <c r="H37" t="s">
+      <c r="M37" t="s">
         <v>55</v>
       </c>
-      <c r="I37" t="s">
-        <v>59</v>
-      </c>
-      <c r="J37" t="s">
-        <v>18</v>
-      </c>
-      <c r="K37" t="s">
-        <v>60</v>
-      </c>
-      <c r="L37" t="s">
-        <v>68</v>
-      </c>
-      <c r="M37" t="s">
-        <v>67</v>
-      </c>
       <c r="N37" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="38" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C38" s="2" t="e">
         <f>AVERAGE(Instance[Newtonsoft])</f>
@@ -1546,7 +1548,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="E38" s="2" t="e">
-        <f>AVERAGE(Instance[fastJSON])</f>
+        <f>AVERAGE(Instance[ProtoBuf (binary reference)])</f>
         <v>#DIV/0!</v>
       </c>
       <c r="F38" s="2" t="e">
@@ -1566,11 +1568,11 @@
         <v>#DIV/0!</v>
       </c>
       <c r="J38" s="2" t="e">
-        <f>AVERAGE(Instance[DSL Platform Java])</f>
+        <f>AVERAGE(Instance[DSL-JSON])</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K38" s="2" t="e">
-        <f>AVERAGE(Instance[Genson])</f>
+        <f>AVERAGE(Instance[Kryo (binary reference)])</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L38" s="2" t="e">
@@ -1602,7 +1604,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="E39" s="2" t="e">
-        <f>AVERAGE(Serialization[fastJSON]) - E38</f>
+        <f>AVERAGE(Serialization[ProtoBuf (binary reference)]) - E38</f>
         <v>#DIV/0!</v>
       </c>
       <c r="F39" s="2" t="e">
@@ -1622,11 +1624,11 @@
         <v>#DIV/0!</v>
       </c>
       <c r="J39" s="2" t="e">
-        <f>AVERAGE(Serialization[DSL Platform Java]) - J38</f>
+        <f>AVERAGE(Serialization[DSL-JSON]) - J38</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K39" s="2" t="e">
-        <f>AVERAGE(Serialization[Genson]) - K38</f>
+        <f>AVERAGE(Serialization[Kryo (binary reference)]) - K38</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L39" s="2" t="e">
@@ -1703,7 +1705,7 @@
     </row>
     <row r="41" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C41" s="2" t="e">
         <f>AVERAGE(Both[Newtonsoft])</f>
@@ -1714,7 +1716,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="E41" s="2" t="e">
-        <f>AVERAGE(Both[fastJSON])</f>
+        <f>AVERAGE(Both[ProtoBuf (binary reference)])</f>
         <v>#DIV/0!</v>
       </c>
       <c r="F41" s="2" t="e">
@@ -1734,11 +1736,11 @@
         <v>#DIV/0!</v>
       </c>
       <c r="J41" s="2" t="e">
-        <f>AVERAGE(Both[DSL Platform Java])</f>
+        <f>AVERAGE(Both[DSL-JSON])</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K41" s="2" t="e">
-        <f>AVERAGE(Both[Genson])</f>
+        <f>AVERAGE(Both[Kryo (binary reference)])</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L41" s="2" t="e">
@@ -1770,7 +1772,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="E42" s="3" t="e">
-        <f>AVERAGE(Serialization[fastJSON (size)])</f>
+        <f>AVERAGE(Serialization[ProtoBuf (size)])</f>
         <v>#DIV/0!</v>
       </c>
       <c r="F42" s="3" t="e">
@@ -1790,11 +1792,11 @@
         <v>#DIV/0!</v>
       </c>
       <c r="J42" s="2" t="e">
-        <f>AVERAGE(Serialization[DSL Platform Java (size)])</f>
+        <f>AVERAGE(Serialization[DSL-JSON (size)])</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K42" s="2" t="e">
-        <f>AVERAGE(Serialization[Genson (size)])</f>
+        <f>AVERAGE(Serialization[Kryo (size)])</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L42" s="2" t="e">
@@ -1833,34 +1835,34 @@
         <v>17</v>
       </c>
       <c r="E46" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="F46" t="s">
         <v>12</v>
       </c>
       <c r="G46" t="s">
+        <v>51</v>
+      </c>
+      <c r="H46" t="s">
+        <v>50</v>
+      </c>
+      <c r="I46" t="s">
+        <v>54</v>
+      </c>
+      <c r="J46" t="s">
+        <v>67</v>
+      </c>
+      <c r="K46" t="s">
+        <v>74</v>
+      </c>
+      <c r="L46" t="s">
         <v>56</v>
       </c>
-      <c r="H46" t="s">
+      <c r="M46" t="s">
         <v>55</v>
       </c>
-      <c r="I46" t="s">
-        <v>59</v>
-      </c>
-      <c r="J46" t="s">
-        <v>18</v>
-      </c>
-      <c r="K46" t="s">
-        <v>60</v>
-      </c>
-      <c r="L46" t="s">
-        <v>68</v>
-      </c>
-      <c r="M46" t="s">
-        <v>67</v>
-      </c>
       <c r="N46" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="47" spans="2:17" x14ac:dyDescent="0.25">
@@ -1876,7 +1878,7 @@
         <v>#NUM!</v>
       </c>
       <c r="E47" s="2" t="e">
-        <f>DEVSQ(Serialization[fastJSON])</f>
+        <f>DEVSQ(Serialization[ProtoBuf (binary reference)])</f>
         <v>#NUM!</v>
       </c>
       <c r="F47" s="2" t="e">
@@ -1896,11 +1898,11 @@
         <v>#NUM!</v>
       </c>
       <c r="J47" s="2" t="e">
-        <f>DEVSQ(Serialization[DSL Platform Java])</f>
+        <f>DEVSQ(Serialization[DSL-JSON])</f>
         <v>#NUM!</v>
       </c>
       <c r="K47" s="2" t="e">
-        <f>DEVSQ(Serialization[Genson])</f>
+        <f>DEVSQ(Serialization[Kryo (binary reference)])</f>
         <v>#NUM!</v>
       </c>
       <c r="L47" s="2" t="e">
@@ -1921,7 +1923,7 @@
     </row>
     <row r="48" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C48" s="2" t="e">
         <f>DEVSQ(Both[Newtonsoft])</f>
@@ -1932,7 +1934,7 @@
         <v>#NUM!</v>
       </c>
       <c r="E48" s="2" t="e">
-        <f>DEVSQ(Both[fastJSON])</f>
+        <f>DEVSQ(Both[ProtoBuf (binary reference)])</f>
         <v>#NUM!</v>
       </c>
       <c r="F48" s="2" t="e">
@@ -1952,11 +1954,11 @@
         <v>#NUM!</v>
       </c>
       <c r="J48" s="2" t="e">
-        <f>DEVSQ(Both[DSL Platform Java])</f>
+        <f>DEVSQ(Both[DSL-JSON])</f>
         <v>#NUM!</v>
       </c>
       <c r="K48" s="2" t="e">
-        <f>DEVSQ(Both[Genson])</f>
+        <f>DEVSQ(Both[Kryo (binary reference)])</f>
         <v>#NUM!</v>
       </c>
       <c r="L48" s="2" t="e">
@@ -1995,72 +1997,72 @@
         <v>17</v>
       </c>
       <c r="D51" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E51" t="s">
         <v>12</v>
       </c>
       <c r="F51" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="G51" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H51" t="s">
         <v>6</v>
       </c>
       <c r="I51" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="J51" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="K51" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="L51" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="M51" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="52" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
+        <v>18</v>
+      </c>
+      <c r="C52" t="s">
         <v>19</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D52" t="s">
+        <v>81</v>
+      </c>
+      <c r="E52" t="s">
         <v>20</v>
       </c>
-      <c r="D52" t="s">
-        <v>69</v>
-      </c>
-      <c r="E52" t="s">
+      <c r="F52" t="s">
         <v>21</v>
       </c>
-      <c r="F52" t="s">
-        <v>22</v>
-      </c>
       <c r="G52" t="s">
+        <v>23</v>
+      </c>
+      <c r="H52" t="s">
         <v>24</v>
       </c>
-      <c r="H52" t="s">
+      <c r="I52" t="s">
+        <v>68</v>
+      </c>
+      <c r="J52" t="s">
+        <v>82</v>
+      </c>
+      <c r="K52" t="s">
+        <v>59</v>
+      </c>
+      <c r="L52" t="s">
+        <v>60</v>
+      </c>
+      <c r="M52" t="s">
         <v>25</v>
-      </c>
-      <c r="I52" t="s">
-        <v>26</v>
-      </c>
-      <c r="J52" t="s">
-        <v>64</v>
-      </c>
-      <c r="K52" t="s">
-        <v>76</v>
-      </c>
-      <c r="L52" t="s">
-        <v>77</v>
-      </c>
-      <c r="M52" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="54" spans="2:25" x14ac:dyDescent="0.25">
@@ -2076,144 +2078,144 @@
         <v>17</v>
       </c>
       <c r="D55" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E55" t="s">
         <v>12</v>
       </c>
       <c r="F55" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="G55" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H55" t="s">
         <v>6</v>
       </c>
       <c r="I55" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="J55" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="K55" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="L55" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="M55" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N55" t="s">
         <v>5</v>
       </c>
       <c r="O55" t="s">
+        <v>35</v>
+      </c>
+      <c r="P55" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q55" t="s">
         <v>38</v>
       </c>
-      <c r="P55" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q55" t="s">
+      <c r="R55" t="s">
+        <v>40</v>
+      </c>
+      <c r="S55" t="s">
         <v>41</v>
-      </c>
-      <c r="R55" t="s">
-        <v>43</v>
-      </c>
-      <c r="S55" t="s">
-        <v>44</v>
       </c>
       <c r="T55" t="s">
         <v>7</v>
       </c>
       <c r="U55" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
       <c r="V55" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="W55" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="X55" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="Y55" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="56" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C56" t="s">
+        <v>34</v>
+      </c>
+      <c r="D56" t="s">
+        <v>80</v>
+      </c>
+      <c r="E56" t="s">
         <v>37</v>
       </c>
-      <c r="D56" t="s">
-        <v>70</v>
-      </c>
-      <c r="E56" t="s">
-        <v>40</v>
-      </c>
       <c r="F56" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="G56" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="H56" t="s">
         <v>8</v>
       </c>
       <c r="I56" t="s">
+        <v>69</v>
+      </c>
+      <c r="J56" t="s">
+        <v>79</v>
+      </c>
+      <c r="K56" t="s">
+        <v>61</v>
+      </c>
+      <c r="L56" t="s">
+        <v>62</v>
+      </c>
+      <c r="M56" t="s">
+        <v>42</v>
+      </c>
+      <c r="N56" t="s">
+        <v>33</v>
+      </c>
+      <c r="O56" t="s">
+        <v>36</v>
+      </c>
+      <c r="P56" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q56" t="s">
+        <v>39</v>
+      </c>
+      <c r="R56" t="s">
         <v>45</v>
       </c>
-      <c r="J56" t="s">
-        <v>63</v>
-      </c>
-      <c r="K56" t="s">
-        <v>78</v>
-      </c>
-      <c r="L56" t="s">
-        <v>79</v>
-      </c>
-      <c r="M56" t="s">
-        <v>46</v>
-      </c>
-      <c r="N56" t="s">
-        <v>36</v>
-      </c>
-      <c r="O56" t="s">
-        <v>39</v>
-      </c>
-      <c r="P56" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q56" t="s">
-        <v>42</v>
-      </c>
-      <c r="R56" t="s">
-        <v>50</v>
-      </c>
       <c r="S56" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="T56" t="s">
         <v>9</v>
       </c>
       <c r="U56" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="V56" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="W56" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="X56" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="Y56" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="58" spans="2:25" x14ac:dyDescent="0.25">
@@ -2229,72 +2231,72 @@
         <v>17</v>
       </c>
       <c r="D59" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E59" t="s">
         <v>12</v>
       </c>
       <c r="F59" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="G59" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H59" t="s">
         <v>6</v>
       </c>
       <c r="I59" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="J59" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="K59" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="L59" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="M59" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="60" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
+        <v>26</v>
+      </c>
+      <c r="C60" t="s">
+        <v>27</v>
+      </c>
+      <c r="D60" t="s">
+        <v>84</v>
+      </c>
+      <c r="E60" t="s">
         <v>28</v>
       </c>
-      <c r="C60" t="s">
+      <c r="F60" t="s">
         <v>29</v>
       </c>
-      <c r="D60" t="s">
-        <v>71</v>
-      </c>
-      <c r="E60" t="s">
+      <c r="G60" t="s">
         <v>30</v>
-      </c>
-      <c r="F60" t="s">
-        <v>31</v>
-      </c>
-      <c r="G60" t="s">
-        <v>32</v>
       </c>
       <c r="H60" t="s">
         <v>10</v>
       </c>
       <c r="I60" t="s">
-        <v>33</v>
+        <v>70</v>
       </c>
       <c r="J60" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="K60" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="L60" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="M60" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>